<commit_message>
Added test methods in Disputes test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-admin.xlsx
+++ b/Web/coyni/resources/testdata-admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(06-09-2022)[2]\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(13-09-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682ED003-2860-4257-8A7C-E22E7665AD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF15A03A-6749-4920-9C95-18C02806D19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coyniPortal" sheetId="2" r:id="rId1"/>
@@ -21,14 +21,16 @@
     <sheet name="checkOut" sheetId="20" r:id="rId6"/>
     <sheet name="Login" sheetId="3" r:id="rId7"/>
     <sheet name="ForgotPassword" sheetId="4" r:id="rId8"/>
-    <sheet name="forgotEmail" sheetId="6" r:id="rId9"/>
-    <sheet name="AddSignetAccount" sheetId="9" r:id="rId10"/>
-    <sheet name="feeStructure" sheetId="10" r:id="rId11"/>
-    <sheet name="TransactionDetails" sheetId="13" r:id="rId12"/>
-    <sheet name="AccountLimits" sheetId="16" r:id="rId13"/>
-    <sheet name="transaction" sheetId="14" r:id="rId14"/>
-    <sheet name="featureControl" sheetId="11" r:id="rId15"/>
-    <sheet name="BalanceReport" sheetId="12" r:id="rId16"/>
+    <sheet name="gobalSearch" sheetId="21" r:id="rId9"/>
+    <sheet name="forgotEmail" sheetId="6" r:id="rId10"/>
+    <sheet name="AddSignetAccount" sheetId="9" r:id="rId11"/>
+    <sheet name="feeStructure" sheetId="10" r:id="rId12"/>
+    <sheet name="TransactionDetails" sheetId="13" r:id="rId13"/>
+    <sheet name="AccountLimits" sheetId="16" r:id="rId14"/>
+    <sheet name="transaction" sheetId="14" r:id="rId15"/>
+    <sheet name="featureControl" sheetId="11" r:id="rId16"/>
+    <sheet name="BalanceReport" sheetId="12" r:id="rId17"/>
+    <sheet name="Disputes" sheetId="22" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="584">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1417,10 +1419,6 @@
     <t>Passwords do not match</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirm Password is required
-</t>
-  </si>
-  <si>
     <t>Admin@321</t>
   </si>
   <si>
@@ -1452,9 +1450,6 @@
   </si>
   <si>
     <t>Crop Your Image</t>
-  </si>
-  <si>
-    <t>images</t>
   </si>
   <si>
     <t>demo.jpg</t>
@@ -1485,12 +1480,6 @@
     <t>Open New Chargeback</t>
   </si>
   <si>
-    <t>08/25/2022</t>
-  </si>
-  <si>
-    <t>08/28/2022</t>
-  </si>
-  <si>
     <t>STATUS,CUSTOMER NAME,ACCOUNT ID,RECEIVED,DUE DATE,CREATED,CBK AMOUNT</t>
   </si>
   <si>
@@ -1596,9 +1585,6 @@
     <t>Remove Profile Image</t>
   </si>
   <si>
-    <t xml:space="preserve"> Are you sure you want to remove your profile image?We will replace it with your initials as a default.</t>
-  </si>
-  <si>
     <t>Success!</t>
   </si>
   <si>
@@ -1632,18 +1618,12 @@
     <t>https://checkout-qa.coyni.com</t>
   </si>
   <si>
-    <t>ravi@outlook.com</t>
-  </si>
-  <si>
     <t>Identity Verification</t>
   </si>
   <si>
     <t>You successfully paid</t>
   </si>
   <si>
-    <t>SOT654876244672</t>
-  </si>
-  <si>
     <t>test checkOut Transaction invalid PopUp</t>
   </si>
   <si>
@@ -1732,13 +1712,115 @@
   </si>
   <si>
     <t>preamount</t>
+  </si>
+  <si>
+    <t>SO23456543245678765123</t>
+  </si>
+  <si>
+    <t>test checkOut module with out adding products</t>
+  </si>
+  <si>
+    <t>Amount is required</t>
+  </si>
+  <si>
+    <t>Empty confirm password</t>
+  </si>
+  <si>
+    <t>Confirm Password is required</t>
+  </si>
+  <si>
+    <t>testGobalSearch</t>
+  </si>
+  <si>
+    <t>Profile ID</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithProfileDetails</t>
+  </si>
+  <si>
+    <t>Profile Details</t>
+  </si>
+  <si>
+    <t>profileDetails</t>
+  </si>
+  <si>
+    <t>test106@gmail.com</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithReferenceID</t>
+  </si>
+  <si>
+    <t>BUT642BC2A2186D577CA521A2C9645C8F</t>
+  </si>
+  <si>
+    <t>09/13/2022</t>
+  </si>
+  <si>
+    <t>09/14/2022</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Are you sure you want to remove your profile image?We will replace it with your initials as a default.</t>
+  </si>
+  <si>
+    <t>customerCountQuery</t>
+  </si>
+  <si>
+    <t>customerBalanceQuery</t>
+  </si>
+  <si>
+    <t>personalBalanceCount</t>
+  </si>
+  <si>
+    <t>businessBalanceQuery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select count(*) from users u where  account_status ='Active'  </t>
+  </si>
+  <si>
+    <t>SELECT sum( total_balance) FROM wallet where wallet_type =0</t>
+  </si>
+  <si>
+    <t>select sum(total_balance)  from users u  inner join wallet w on u.id=w.user_id where u.account_type =1</t>
+  </si>
+  <si>
+    <t>select sum(total_balance)  from users u  inner join wallet w on u.id=w.user_id where u.account_type in (2,6,4)</t>
+  </si>
+  <si>
+    <t>VerifyCountAndBalance</t>
+  </si>
+  <si>
+    <t>filterHeadings</t>
+  </si>
+  <si>
+    <t>caseNum</t>
+  </si>
+  <si>
+    <t>disputesExportsStatusCaseID</t>
+  </si>
+  <si>
+    <t>Verify filters headings</t>
+  </si>
+  <si>
+    <t>Case Number,Customer Name,Account ID,Received Date,Due Date,Created Date,Card First 6,Card Last 4</t>
+  </si>
+  <si>
+    <t>Verify case num filter won dispaly</t>
+  </si>
+  <si>
+    <t>Verify export status case num dispaly</t>
+  </si>
+  <si>
+    <t>Won,12346</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1878,6 +1960,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1915,7 +2003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1961,6 +2049,18 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3092,10 +3192,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>25</v>
@@ -3172,11 +3272,1175 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D341FF-C706-4B03-BBF1-19B6EBC55B3F}">
+  <dimension ref="A1:AC15"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="65.42578125" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" customWidth="1"/>
+    <col min="24" max="24" width="26.42578125" customWidth="1"/>
+    <col min="25" max="25" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V3" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" ht="39" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V6" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V7" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X7" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V8" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X8" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V9" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X9" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V10" s="2">
+        <v>333333</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X10" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V11" s="2">
+        <v>123</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X11" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1234567</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X12" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V13" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X13" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V14" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X14" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+    </row>
+    <row r="15" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="V15" s="2">
+        <v>123456</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X15" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E3168F23-BB22-441E-BE39-6AB195ABA385}"/>
+    <hyperlink ref="D3:D15" r:id="rId2" display="Santoshp@ideyalabs.com" xr:uid="{BFF184B9-64B8-4CF8-AB68-F3F9D9C5E528}"/>
+    <hyperlink ref="S2" r:id="rId3" xr:uid="{E3DF655E-0800-4E81-9F4A-F1675585BC9C}"/>
+    <hyperlink ref="S3:S15" r:id="rId4" display="Santoshp@ideyalabs.com" xr:uid="{0F22233D-4069-4DD3-9CEE-46D40E3AC408}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B0A0B3-8637-430C-83AB-3CD1E7890F66}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,7 +4722,7 @@
       </c>
       <c r="W4" s="20"/>
       <c r="Y4" t="s">
-        <v>383</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="45" x14ac:dyDescent="0.25">
@@ -3773,9 +5037,7 @@
       <c r="S9" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="T9" s="15">
-        <v>125</v>
-      </c>
+      <c r="T9" s="15"/>
       <c r="U9" s="17" t="s">
         <v>286</v>
       </c>
@@ -3875,7 +5137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D290E486-9137-49B5-9733-BAB7620F9D07}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -4161,12 +5423,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B863EE-0FB8-4125-A633-87E6E4517058}">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4250,34 +5512,34 @@
         <v>314</v>
       </c>
       <c r="R1" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>485</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>178</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>16</v>
@@ -4583,10 +5845,10 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>25</v>
@@ -4622,39 +5884,39 @@
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="S8">
         <v>12346</v>
       </c>
       <c r="T8" s="29" t="s">
+        <v>563</v>
+      </c>
+      <c r="U8" s="29" t="s">
+        <v>564</v>
+      </c>
+      <c r="V8" t="s">
+        <v>472</v>
+      </c>
+      <c r="W8" t="s">
+        <v>473</v>
+      </c>
+      <c r="X8" t="s">
         <v>474</v>
       </c>
-      <c r="U8" s="29" t="s">
+      <c r="Y8" t="s">
         <v>475</v>
       </c>
-      <c r="V8" t="s">
+      <c r="Z8" t="s">
         <v>476</v>
-      </c>
-      <c r="W8" t="s">
-        <v>477</v>
-      </c>
-      <c r="X8" t="s">
-        <v>478</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>479</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>25</v>
@@ -4684,15 +5946,15 @@
         <v>33</v>
       </c>
       <c r="AA9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>25</v>
@@ -4722,7 +5984,7 @@
         <v>33</v>
       </c>
       <c r="AB10" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4746,7 +6008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6996C0C-24E0-40BE-A97F-7A279690A8EE}">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -5005,7 +6267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DAABDA-3594-43D7-9AEC-0D8E440ACE4D}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
@@ -5112,7 +6374,7 @@
         <v>16</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>178</v>
@@ -5170,7 +6432,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="15"/>
       <c r="Y2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5549,7 +6811,7 @@
     </row>
     <row r="10" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>64</v>
@@ -5594,7 +6856,7 @@
       <c r="V10" s="15"/>
       <c r="W10" s="15"/>
       <c r="X10" s="16" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -5622,7 +6884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B6D706-4369-43B1-B41D-E358306B83B4}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -5735,12 +6997,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9ECCE6-1FC9-48C7-BBB8-F3E55C223DFA}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5751,15 +7013,19 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.7109375" customWidth="1"/>
+    <col min="16" max="16" width="33.140625" customWidth="1"/>
+    <col min="17" max="17" width="33.28515625" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5796,16 +7062,28 @@
       <c r="L1" t="s">
         <v>354</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="22" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="22" t="s">
+        <v>567</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>575</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -5826,7 +7104,7 @@
         <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
@@ -5834,13 +7112,23 @@
       <c r="J2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2" s="6"/>
+      <c r="O2" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>573</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -5861,7 +7149,7 @@
         <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
@@ -5870,16 +7158,14 @@
         <v>32</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="33"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>359</v>
       </c>
@@ -5887,7 +7173,7 @@
         <v>130</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -5902,7 +7188,7 @@
         <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
         <v>31</v>
@@ -5914,16 +7200,13 @@
         <v>50</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -5931,7 +7214,7 @@
         <v>130</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -5946,7 +7229,7 @@
         <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
         <v>31</v>
@@ -5964,10 +7247,10 @@
         <v>361</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>359</v>
       </c>
@@ -5975,7 +7258,7 @@
         <v>130</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -5990,7 +7273,7 @@
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
@@ -6008,10 +7291,280 @@
         <v>361</v>
       </c>
       <c r="N6" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>359</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>365</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7608AE-4E83-4A59-A303-21D2C67D6F9E}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>580</v>
+      </c>
+      <c r="M2" s="35"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2">
+        <v>123456</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35">
+        <v>12346</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35">
+        <v>12346</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="mailto:santoshp@ideyalabs.com" xr:uid="{D8142083-A2AC-4CA1-969E-3A847814A02A}"/>
+    <hyperlink ref="E2" r:id="rId2" display="mailto:Admin@123" xr:uid="{A6C76653-F138-4D91-A2DD-DB2DB59B3651}"/>
+    <hyperlink ref="D3" r:id="rId3" display="mailto:santoshp@ideyalabs.com" xr:uid="{E9181E14-5E7D-4609-BBA6-1C62CF8B3FCA}"/>
+    <hyperlink ref="E3" r:id="rId4" display="mailto:Admin@123" xr:uid="{A078E4AC-2FB0-4E82-ACB2-2843AE63D96F}"/>
+    <hyperlink ref="D4" r:id="rId5" display="mailto:santoshp@ideyalabs.com" xr:uid="{14E9D234-28F9-45C7-90B0-A7AFAF91B064}"/>
+    <hyperlink ref="E4" r:id="rId6" display="mailto:Admin@123" xr:uid="{8E11D7EC-539F-416A-9C0F-2B1D8BB166D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7115,13 +8668,13 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
@@ -7315,12 +8868,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>450</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>450</v>
+        <v>553</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>69</v>
@@ -7349,8 +8902,8 @@
       <c r="K5" t="s">
         <v>451</v>
       </c>
-      <c r="M5" s="26" t="s">
-        <v>454</v>
+      <c r="M5" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -7385,10 +8938,10 @@
         <v>27</v>
       </c>
       <c r="L6" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="M6" t="s">
         <v>455</v>
-      </c>
-      <c r="M6" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7426,7 +8979,7 @@
         <v>27</v>
       </c>
       <c r="M7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -7435,15 +8988,15 @@
     <hyperlink ref="D2" r:id="rId2" xr:uid="{28730DAE-451E-4056-932E-331C142D8306}"/>
     <hyperlink ref="E3" r:id="rId3" xr:uid="{A08E1913-13F7-48A5-BE6C-957E4F387918}"/>
     <hyperlink ref="E4" r:id="rId4" xr:uid="{E11209F2-6A71-476E-ABA7-9C98D4F93D10}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{61BCD2C3-0FE4-45F2-B33B-D0B703CC47DC}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{6071F8DD-0AB2-418A-A3F6-D1B8A5F08556}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{38A9D038-8E27-4DB0-B9AA-48D104870A0B}"/>
-    <hyperlink ref="D3" r:id="rId8" xr:uid="{CDDBBC93-AB18-48DB-8BD6-BD5DB55D7AF5}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{6D4AE43B-1850-4D70-A4E6-611571069584}"/>
-    <hyperlink ref="D5" r:id="rId10" xr:uid="{B270F226-9075-4A2B-A429-F8DE59CAFE67}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{0DFB2FC0-0E63-482B-BACD-B454EA527BAA}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{C1F0477F-6B25-432F-8647-E5EAFAF9629E}"/>
-    <hyperlink ref="L6" r:id="rId13" xr:uid="{DB74C80E-3532-4617-A493-030E61DAC555}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{6071F8DD-0AB2-418A-A3F6-D1B8A5F08556}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{38A9D038-8E27-4DB0-B9AA-48D104870A0B}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{CDDBBC93-AB18-48DB-8BD6-BD5DB55D7AF5}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{6D4AE43B-1850-4D70-A4E6-611571069584}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{0DFB2FC0-0E63-482B-BACD-B454EA527BAA}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{C1F0477F-6B25-432F-8647-E5EAFAF9629E}"/>
+    <hyperlink ref="L6" r:id="rId11" xr:uid="{DB74C80E-3532-4617-A493-030E61DAC555}"/>
+    <hyperlink ref="E5" r:id="rId12" xr:uid="{6C64FE84-8DEF-4E93-B32D-F4DD9447C021}"/>
+    <hyperlink ref="D5" r:id="rId13" xr:uid="{CC6B220E-F8B1-43B6-A2D2-3E62AC6398D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7454,7 +9007,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7513,25 +9066,25 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>178</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>10</v>
@@ -7539,10 +9092,10 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" t="s">
         <v>462</v>
-      </c>
-      <c r="B2" t="s">
-        <v>463</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>25</v>
@@ -7572,30 +9125,30 @@
         <v>33</v>
       </c>
       <c r="L2" s="15" t="s">
+        <v>463</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>464</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="O2" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>467</v>
-      </c>
       <c r="R2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="S2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B3" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>25</v>
@@ -7625,13 +9178,13 @@
         <v>33</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>511</v>
+        <v>566</v>
       </c>
       <c r="Q3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -7647,10 +9200,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFB9E42-5696-4F0E-9E81-9692429FA356}">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7690,16 +9243,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -7717,37 +9270,37 @@
         <v>443</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>178</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>334</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>270</v>
@@ -7765,78 +9318,78 @@
         <v>273</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E2" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="F2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="S2" s="15" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="U2" s="31" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="W2" s="31">
         <v>151</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>284</v>
@@ -7848,7 +9401,7 @@
         <v>285</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="AD2">
         <v>1.01</v>
@@ -7856,69 +9409,89 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="B3" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E3" t="s">
-        <v>526</v>
+        <v>550</v>
       </c>
       <c r="F3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G3" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B4" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E4" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="F4" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G4" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="K4" s="20" t="s">
         <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="N4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="O4" t="s">
-        <v>534</v>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="B5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="F5" t="s">
+        <v>515</v>
+      </c>
+      <c r="G5" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -7927,12 +9500,13 @@
     <hyperlink ref="I2" r:id="rId2" xr:uid="{3AC1157B-CBFE-4A3A-97F2-CD1BA069B9E6}"/>
     <hyperlink ref="D3" r:id="rId3" xr:uid="{D6C2FFC5-EEDC-4E5E-8437-BA3012C285EE}"/>
     <hyperlink ref="D4" r:id="rId4" xr:uid="{A4D159C9-78DA-46E9-AAA2-6DE96443BDF7}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{FD28FB94-76D7-4821-9E85-BA88C8C348FE}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{D01AE455-D8CC-4FA6-BD42-D57F16011A5B}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{372C5DDD-5BB6-4E59-A318-BC1678609099}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{D01AE455-D8CC-4FA6-BD42-D57F16011A5B}"/>
+    <hyperlink ref="H2" r:id="rId6" xr:uid="{372C5DDD-5BB6-4E59-A318-BC1678609099}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{FB91854F-486D-427A-88C7-1F44420EB6D5}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{796B7C4B-5468-4CB8-AB33-9A2C92038486}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -8016,10 +9590,10 @@
         <v>128</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -8492,16 +10066,16 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>27</v>
@@ -8510,24 +10084,24 @@
         <v>28</v>
       </c>
       <c r="Q15" s="30" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="R15" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>27</v>
@@ -8536,10 +10110,10 @@
         <v>28</v>
       </c>
       <c r="Q16" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="R16" t="s">
         <v>491</v>
-      </c>
-      <c r="R16" t="s">
-        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -8562,8 +10136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C474AF-1560-47F8-90E0-FD2FFD96A555}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9163,7 +10737,7 @@
       <c r="K11" s="2">
         <v>112121</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="9" t="s">
         <v>148</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -9337,39 +10911,37 @@
     <hyperlink ref="D7:D14" r:id="rId12" display="Santoshp@ideyalabs.com" xr:uid="{825E4587-EEF3-49C5-A0DC-7C972BBF1E33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D341FF-C706-4B03-BBF1-19B6EBC55B3F}">
-  <dimension ref="A1:AC15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77806F8-4095-4D16-96F4-6911E0B4577F}">
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="74.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="65.42578125" customWidth="1"/>
-    <col min="16" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="86" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.140625" customWidth="1"/>
-    <col min="23" max="23" width="17.85546875" customWidth="1"/>
-    <col min="24" max="24" width="26.42578125" customWidth="1"/>
-    <col min="25" max="25" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -9388,10 +10960,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -9403,1103 +10975,140 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>218</v>
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>559</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V2" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="2" t="s">
+      <c r="E2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>69</v>
+      <c r="L2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V3" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC3" s="2"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="E3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V4" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC4" s="2"/>
-    </row>
-    <row r="5" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V5" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X5" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC5" s="2"/>
-    </row>
-    <row r="6" spans="1:29" ht="39" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y6" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="AC6" s="2"/>
-    </row>
-    <row r="7" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V7" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X7" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="AC7" s="2"/>
-    </row>
-    <row r="8" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V8" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W8" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X8" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z8" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="AC8" s="2"/>
-    </row>
-    <row r="9" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="S9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V9" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X9" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-    </row>
-    <row r="10" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V10" s="2">
-        <v>333333</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X10" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V11" s="2">
-        <v>123</v>
-      </c>
-      <c r="W11" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X11" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V12" s="2">
-        <v>1234567</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X12" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V13" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W13" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X13" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-    </row>
-    <row r="14" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V14" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W14" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X14" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-    </row>
-    <row r="15" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="S15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="V15" s="2">
-        <v>123456</v>
-      </c>
-      <c r="W15" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="X15" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="2"/>
+      <c r="E4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" t="s">
+        <v>562</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E3168F23-BB22-441E-BE39-6AB195ABA385}"/>
-    <hyperlink ref="D3:D15" r:id="rId2" display="Santoshp@ideyalabs.com" xr:uid="{BFF184B9-64B8-4CF8-AB68-F3F9D9C5E528}"/>
-    <hyperlink ref="S2" r:id="rId3" xr:uid="{E3DF655E-0800-4E81-9F4A-F1675585BC9C}"/>
-    <hyperlink ref="S3:S15" r:id="rId4" display="Santoshp@ideyalabs.com" xr:uid="{0F22233D-4069-4DD3-9CEE-46D40E3AC408}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{47A8E0C1-C045-410B-870A-6113AA235D59}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{995B17B2-19C4-4940-B846-AE79A09D03ED}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{25A957EB-4F77-45D7-A75A-30E825B6985A}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{E5910FB0-36E0-4AD3-BAC7-06236F498B91}"/>
+    <hyperlink ref="M3" r:id="rId5" xr:uid="{C49D242B-2EF9-40FF-B1F8-8653F1F4387D}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{6B3C10D3-8DD9-4A3E-B426-A83A0A2F8221}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{EB1D00DE-69F3-42BF-9D29-33A8F2724E26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sanity test suite for Admin portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-admin.xlsx
+++ b/Web/coyni/resources/testdata-admin.xlsx
@@ -1,41 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\admin(27-12-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BF92C9-F713-4A0C-92B7-A091C88DF3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9558649-9895-41AA-A7B8-8A47BC4C8C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="10455" windowHeight="9180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coyniPortal" sheetId="2" r:id="rId1"/>
     <sheet name="accounting" sheetId="15" r:id="rId2"/>
-    <sheet name="profiles" sheetId="17" r:id="rId3"/>
-    <sheet name="profilesIndividuals" sheetId="24" r:id="rId4"/>
-    <sheet name="underWritings" sheetId="23" r:id="rId5"/>
-    <sheet name="SignupPageMerchant" sheetId="27" r:id="rId6"/>
-    <sheet name="changePassword" sheetId="18" r:id="rId7"/>
-    <sheet name="userDetails" sheetId="19" r:id="rId8"/>
-    <sheet name="checkOut" sheetId="20" r:id="rId9"/>
-    <sheet name="Login" sheetId="3" r:id="rId10"/>
-    <sheet name="exportFile" sheetId="25" r:id="rId11"/>
-    <sheet name="ForgotPassword" sheetId="4" r:id="rId12"/>
-    <sheet name="gobalSearch" sheetId="21" r:id="rId13"/>
-    <sheet name="forgotEmail" sheetId="6" r:id="rId14"/>
-    <sheet name="AddCogentAccount" sheetId="9" r:id="rId15"/>
-    <sheet name="SignupPage" sheetId="26" r:id="rId16"/>
-    <sheet name="feeStructure" sheetId="10" r:id="rId17"/>
-    <sheet name="TransactionDetails" sheetId="13" r:id="rId18"/>
-    <sheet name="AccountLimits" sheetId="16" r:id="rId19"/>
-    <sheet name="transaction" sheetId="14" r:id="rId20"/>
-    <sheet name="featureControl" sheetId="11" r:id="rId21"/>
-    <sheet name="BalanceReport" sheetId="12" r:id="rId22"/>
-    <sheet name="Disputes" sheetId="22" r:id="rId23"/>
+    <sheet name="gatewaySettings" sheetId="28" r:id="rId3"/>
+    <sheet name="profiles" sheetId="17" r:id="rId4"/>
+    <sheet name="profilesIndividuals" sheetId="24" r:id="rId5"/>
+    <sheet name="underWritings" sheetId="23" r:id="rId6"/>
+    <sheet name="SignupPageMerchant" sheetId="27" r:id="rId7"/>
+    <sheet name="changePassword" sheetId="18" r:id="rId8"/>
+    <sheet name="userDetails" sheetId="19" r:id="rId9"/>
+    <sheet name="checkOut" sheetId="20" r:id="rId10"/>
+    <sheet name="Login" sheetId="3" r:id="rId11"/>
+    <sheet name="exportFile" sheetId="25" r:id="rId12"/>
+    <sheet name="ForgotPassword" sheetId="4" r:id="rId13"/>
+    <sheet name="gobalSearch" sheetId="21" r:id="rId14"/>
+    <sheet name="forgotEmail" sheetId="6" r:id="rId15"/>
+    <sheet name="AddCogentAccount" sheetId="9" r:id="rId16"/>
+    <sheet name="SignupPage" sheetId="26" r:id="rId17"/>
+    <sheet name="feeStructure" sheetId="10" r:id="rId18"/>
+    <sheet name="TransactionDetails" sheetId="13" r:id="rId19"/>
+    <sheet name="AccountLimits" sheetId="16" r:id="rId20"/>
+    <sheet name="transaction" sheetId="14" r:id="rId21"/>
+    <sheet name="featureControl" sheetId="11" r:id="rId22"/>
+    <sheet name="BalanceReport" sheetId="12" r:id="rId23"/>
+    <sheet name="Disputes" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3714" uniqueCount="853">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2582,6 +2583,69 @@
   </si>
   <si>
     <t>Test Debit</t>
+  </si>
+  <si>
+    <t>Admin login Page With links</t>
+  </si>
+  <si>
+    <t>test verify user details links</t>
+  </si>
+  <si>
+    <t>testProfilewithPersonalMerchant</t>
+  </si>
+  <si>
+    <t>Verify Underwriting Links</t>
+  </si>
+  <si>
+    <t>ApiHeading</t>
+  </si>
+  <si>
+    <t>Underwriting - API Business</t>
+  </si>
+  <si>
+    <t>Verify reserve mgmt</t>
+  </si>
+  <si>
+    <t>Reserves</t>
+  </si>
+  <si>
+    <t>test disputes tests</t>
+  </si>
+  <si>
+    <t>disputesHeading</t>
+  </si>
+  <si>
+    <t>Disputes</t>
+  </si>
+  <si>
+    <t>test Accounting</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>loadBalancer</t>
+  </si>
+  <si>
+    <t>paymenyMethod</t>
+  </si>
+  <si>
+    <t>Payment Gateways</t>
+  </si>
+  <si>
+    <t>Load Balancer</t>
+  </si>
+  <si>
+    <t>test GateWay settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify exportFile </t>
+  </si>
+  <si>
+    <t>Exported Files</t>
+  </si>
+  <si>
+    <t>VerifyBalanceReportTest</t>
   </si>
 </sst>
 </file>
@@ -2818,7 +2882,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2837,8 +2901,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2855,13 +2925,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2983,6 +3068,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4261,11 +4351,323 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFB9E42-5696-4F0E-9E81-9692429FA356}">
+  <dimension ref="A1:AD5"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="111.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="109" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="E2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G2" t="s">
+        <v>541</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>474</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>475</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>487</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="V2" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="W2" s="57" t="s">
+        <v>803</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="E3" t="s">
+        <v>506</v>
+      </c>
+      <c r="F3" t="s">
+        <v>471</v>
+      </c>
+      <c r="G3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>478</v>
+      </c>
+      <c r="B4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="E4" t="s">
+        <v>484</v>
+      </c>
+      <c r="F4" t="s">
+        <v>471</v>
+      </c>
+      <c r="G4" t="s">
+        <v>472</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>474</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>479</v>
+      </c>
+      <c r="N4" t="s">
+        <v>482</v>
+      </c>
+      <c r="O4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>507</v>
+      </c>
+      <c r="B5" t="s">
+        <v>479</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="F5" t="s">
+        <v>471</v>
+      </c>
+      <c r="G5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E514FC88-A5B1-4E65-87FF-7CADA1E00A73}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{3AC1157B-CBFE-4A3A-97F2-CD1BA069B9E6}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{D6C2FFC5-EEDC-4E5E-8437-BA3012C285EE}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{A4D159C9-78DA-46E9-AAA2-6DE96443BDF7}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{D01AE455-D8CC-4FA6-BD42-D57F16011A5B}"/>
+    <hyperlink ref="H2" r:id="rId6" xr:uid="{372C5DDD-5BB6-4E59-A318-BC1678609099}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{FB91854F-486D-427A-88C7-1F44420EB6D5}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{796B7C4B-5468-4CB8-AB33-9A2C92038486}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB4A103-5E7C-460B-A3AA-C11BE99C8FB4}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,9 +4693,11 @@
     <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" customWidth="1"/>
     <col min="23" max="23" width="52" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4363,8 +4767,14 @@
       <c r="W1" s="22" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>109</v>
       </c>
@@ -4409,7 +4819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
@@ -4444,7 +4854,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>112</v>
       </c>
@@ -4479,7 +4889,7 @@
       </c>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>112</v>
       </c>
@@ -4516,7 +4926,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>112</v>
       </c>
@@ -4553,7 +4963,7 @@
       </c>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>123</v>
       </c>
@@ -4598,7 +5008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
@@ -4637,7 +5047,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>125</v>
       </c>
@@ -4676,7 +5086,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -4715,7 +5125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>125</v>
       </c>
@@ -4754,7 +5164,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>125</v>
       </c>
@@ -4793,7 +5203,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>125</v>
       </c>
@@ -4832,7 +5242,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -4871,7 +5281,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>440</v>
       </c>
@@ -4897,7 +5307,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>440</v>
       </c>
@@ -4923,7 +5333,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>774</v>
       </c>
@@ -4949,7 +5359,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>777</v>
       </c>
@@ -4969,7 +5379,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>785</v>
       </c>
@@ -5021,6 +5431,26 @@
       </c>
       <c r="V19" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="73" t="s">
+        <v>832</v>
+      </c>
+      <c r="B20" s="73" t="s">
+        <v>832</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5047,12 +5477,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE7FBCC-0AD2-4CB8-BB75-EACD68A9A988}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J4"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5069,9 +5499,10 @@
     <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5114,13 +5545,16 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>654</v>
-      </c>
-      <c r="B2" t="s">
-        <v>655</v>
+      <c r="O1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>850</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>850</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>25</v>
@@ -5152,13 +5586,16 @@
       <c r="L2">
         <v>123456</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>25</v>
@@ -5190,19 +5627,13 @@
       <c r="L3">
         <v>123456</v>
       </c>
-      <c r="M3" t="s">
-        <v>463</v>
-      </c>
-      <c r="N3" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B4" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>25</v>
@@ -5238,6 +5669,50 @@
         <v>463</v>
       </c>
       <c r="N4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>659</v>
+      </c>
+      <c r="B5" t="s">
+        <v>660</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>123456</v>
+      </c>
+      <c r="M5" t="s">
+        <v>463</v>
+      </c>
+      <c r="N5" t="s">
         <v>661</v>
       </c>
     </row>
@@ -5246,12 +5721,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C474AF-1560-47F8-90E0-FD2FFD96A555}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6039,7 +6514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77806F8-4095-4D16-96F4-6911E0B4577F}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -6250,12 +6725,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D341FF-C706-4B03-BBF1-19B6EBC55B3F}">
   <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7415,7 +7890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B0A0B3-8637-430C-83AB-3CD1E7890F66}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
@@ -8148,7 +8623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77372ADD-3C84-4CC3-8B32-31147894CD0D}">
   <dimension ref="A1:CB2"/>
   <sheetViews>
@@ -8657,7 +9132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D290E486-9137-49B5-9733-BAB7620F9D07}">
   <dimension ref="A1:T10"/>
   <sheetViews>
@@ -9161,7 +9636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B863EE-0FB8-4125-A633-87E6E4517058}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
@@ -9980,7 +10455,679 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDD6E72-6031-4802-B904-6A5DCC120EE9}">
+  <dimension ref="A1:X9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="60"/>
+    <col min="4" max="4" width="23.28515625" style="60" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="60" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="60" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="60" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" style="60" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="60" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="85.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="60"/>
+    <col min="22" max="22" width="26.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="59" t="s">
+        <v>649</v>
+      </c>
+      <c r="X1" s="60" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>843</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>843</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>651</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="65" t="s">
+        <v>805</v>
+      </c>
+      <c r="P3" s="61" t="s">
+        <v>810</v>
+      </c>
+      <c r="Q3" s="61" t="s">
+        <v>815</v>
+      </c>
+      <c r="R3" s="61" t="s">
+        <v>815</v>
+      </c>
+      <c r="S3" s="66" t="s">
+        <v>816</v>
+      </c>
+      <c r="T3" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="64" t="s">
+        <v>806</v>
+      </c>
+      <c r="P4" s="61" t="s">
+        <v>811</v>
+      </c>
+      <c r="Q4" s="64" t="s">
+        <v>817</v>
+      </c>
+      <c r="R4" s="64" t="s">
+        <v>817</v>
+      </c>
+      <c r="S4" s="64" t="s">
+        <v>818</v>
+      </c>
+      <c r="T4" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U4" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="64" t="s">
+        <v>807</v>
+      </c>
+      <c r="P5" s="61" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q5" s="61" t="s">
+        <v>819</v>
+      </c>
+      <c r="R5" s="61" t="s">
+        <v>819</v>
+      </c>
+      <c r="S5" s="61" t="s">
+        <v>820</v>
+      </c>
+      <c r="T5" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U5" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="64" t="s">
+        <v>808</v>
+      </c>
+      <c r="P6" s="61" t="s">
+        <v>813</v>
+      </c>
+      <c r="Q6" s="64" t="s">
+        <v>821</v>
+      </c>
+      <c r="R6" s="61" t="s">
+        <v>821</v>
+      </c>
+      <c r="S6" s="61" t="s">
+        <v>822</v>
+      </c>
+      <c r="T6" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U6" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V6" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="O7" s="64" t="s">
+        <v>823</v>
+      </c>
+      <c r="P7" s="61" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q7" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="R7" s="64" t="s">
+        <v>827</v>
+      </c>
+      <c r="S7" s="61" t="s">
+        <v>820</v>
+      </c>
+      <c r="T7" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V7" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8" s="61" t="s">
+        <v>652</v>
+      </c>
+      <c r="P8" s="61" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q8" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="S8" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V8" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="O9" s="64" t="s">
+        <v>809</v>
+      </c>
+      <c r="P9" s="61" t="s">
+        <v>814</v>
+      </c>
+      <c r="Q9" s="64" t="s">
+        <v>825</v>
+      </c>
+      <c r="R9" s="64" t="s">
+        <v>825</v>
+      </c>
+      <c r="S9" s="61" t="s">
+        <v>826</v>
+      </c>
+      <c r="T9" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="W9" s="62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{92A74E4F-278C-46C5-B56F-1DEE573A2B71}"/>
+    <hyperlink ref="D4:D9" r:id="rId2" display="santoshp@ideyalabs.com" xr:uid="{CC451CFC-3178-411D-8AF5-CDABD2D340D2}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{886819AD-D182-4E9F-BC94-32AA1035B8BD}"/>
+    <hyperlink ref="E4:E9" r:id="rId4" display="Admin@123" xr:uid="{CBF914E0-82B1-46E2-AFA0-E6B23CE0BEE0}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{B37B8191-13A8-4684-B23D-799EFCF09DFD}"/>
+    <hyperlink ref="E2" r:id="rId6" xr:uid="{42802A4C-E267-4B48-B1F8-799622013887}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6996C0C-24E0-40BE-A97F-7A279690A8EE}">
   <dimension ref="A1:P6"/>
   <sheetViews>
@@ -10259,622 +11406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDD6E72-6031-4802-B904-6A5DCC120EE9}">
-  <dimension ref="A1:W8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="60"/>
-    <col min="4" max="4" width="23.28515625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="60" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="60" customWidth="1"/>
-    <col min="7" max="7" width="48.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="60" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="60" customWidth="1"/>
-    <col min="16" max="16" width="26.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="85.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="60"/>
-    <col min="22" max="22" width="26.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="60"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="T1" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="U1" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="W1" s="59" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="30.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="61" t="s">
-        <v>651</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="65" t="s">
-        <v>805</v>
-      </c>
-      <c r="P2" s="61" t="s">
-        <v>810</v>
-      </c>
-      <c r="Q2" s="61" t="s">
-        <v>815</v>
-      </c>
-      <c r="R2" s="61" t="s">
-        <v>815</v>
-      </c>
-      <c r="S2" s="66" t="s">
-        <v>816</v>
-      </c>
-      <c r="T2" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>806</v>
-      </c>
-      <c r="P3" s="61" t="s">
-        <v>811</v>
-      </c>
-      <c r="Q3" s="64" t="s">
-        <v>817</v>
-      </c>
-      <c r="R3" s="64" t="s">
-        <v>817</v>
-      </c>
-      <c r="S3" s="64" t="s">
-        <v>818</v>
-      </c>
-      <c r="T3" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U3" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="O4" s="64" t="s">
-        <v>807</v>
-      </c>
-      <c r="P4" s="61" t="s">
-        <v>812</v>
-      </c>
-      <c r="Q4" s="61" t="s">
-        <v>819</v>
-      </c>
-      <c r="R4" s="61" t="s">
-        <v>819</v>
-      </c>
-      <c r="S4" s="61" t="s">
-        <v>820</v>
-      </c>
-      <c r="T4" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U4" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W4" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="64" t="s">
-        <v>808</v>
-      </c>
-      <c r="P5" s="61" t="s">
-        <v>813</v>
-      </c>
-      <c r="Q5" s="64" t="s">
-        <v>821</v>
-      </c>
-      <c r="R5" s="61" t="s">
-        <v>821</v>
-      </c>
-      <c r="S5" s="61" t="s">
-        <v>822</v>
-      </c>
-      <c r="T5" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U5" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V5" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W5" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="O6" s="64" t="s">
-        <v>823</v>
-      </c>
-      <c r="P6" s="61" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q6" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="R6" s="64" t="s">
-        <v>827</v>
-      </c>
-      <c r="S6" s="61" t="s">
-        <v>820</v>
-      </c>
-      <c r="T6" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U6" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V6" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="O7" s="61" t="s">
-        <v>652</v>
-      </c>
-      <c r="P7" s="61" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q7" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="R7" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="S7" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="T7" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U7" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W7" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="O8" s="64" t="s">
-        <v>809</v>
-      </c>
-      <c r="P8" s="61" t="s">
-        <v>814</v>
-      </c>
-      <c r="Q8" s="64" t="s">
-        <v>825</v>
-      </c>
-      <c r="R8" s="64" t="s">
-        <v>825</v>
-      </c>
-      <c r="S8" s="61" t="s">
-        <v>826</v>
-      </c>
-      <c r="T8" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="U8" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="V8" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="W8" s="62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{92A74E4F-278C-46C5-B56F-1DEE573A2B71}"/>
-    <hyperlink ref="D3:D8" r:id="rId2" display="santoshp@ideyalabs.com" xr:uid="{CC451CFC-3178-411D-8AF5-CDABD2D340D2}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{886819AD-D182-4E9F-BC94-32AA1035B8BD}"/>
-    <hyperlink ref="E3:E8" r:id="rId4" display="Admin@123" xr:uid="{CBF914E0-82B1-46E2-AFA0-E6B23CE0BEE0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DAABDA-3594-43D7-9AEC-0D8E440ACE4D}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
@@ -11522,7 +12054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B6D706-4369-43B1-B41D-E358306B83B4}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -11635,12 +12167,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9ECCE6-1FC9-48C7-BBB8-F3E55C223DFA}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11722,12 +12254,12 @@
         <v>649</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>852</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>852</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>25</v>
@@ -11753,26 +12285,20 @@
       <c r="J2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="O2" s="32" t="s">
-        <v>523</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>525</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>526</v>
-      </c>
+      <c r="K2" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="32"/>
       <c r="S2" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>527</v>
       </c>
       <c r="B3" t="s">
         <v>110</v>
@@ -11801,20 +12327,26 @@
       <c r="J3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="32"/>
+      <c r="K3" s="6"/>
+      <c r="O3" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>525</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>526</v>
+      </c>
       <c r="S3" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
@@ -11844,14 +12376,12 @@
         <v>32</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>333</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="32"/>
       <c r="S4" s="20" t="s">
         <v>32</v>
       </c>
@@ -11864,7 +12394,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -11891,13 +12421,10 @@
         <v>50</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>335</v>
       </c>
       <c r="S5" s="20" t="s">
         <v>32</v>
@@ -11911,7 +12438,7 @@
         <v>110</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -11944,7 +12471,7 @@
         <v>333</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S6" s="20" t="s">
         <v>32</v>
@@ -11958,7 +12485,7 @@
         <v>110</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -11991,9 +12518,56 @@
         <v>333</v>
       </c>
       <c r="N7" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S8" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -12003,12 +12577,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7608AE-4E83-4A59-A303-21D2C67D6F9E}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12075,14 +12649,16 @@
       <c r="O1" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="P1" s="15"/>
-    </row>
-    <row r="2" spans="1:16" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>531</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>531</v>
+      <c r="P1" s="15" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>840</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>840</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>25</v>
@@ -12111,22 +12687,20 @@
       <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="35" t="s">
-        <v>532</v>
-      </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="15"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="15"/>
+      <c r="P2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>25</v>
@@ -12155,10 +12729,10 @@
       <c r="K3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="58" t="s">
-        <v>800</v>
-      </c>
+      <c r="L3" s="35" t="s">
+        <v>532</v>
+      </c>
+      <c r="M3" s="34"/>
       <c r="N3" s="15"/>
       <c r="O3" s="7" t="s">
         <v>32</v>
@@ -12167,10 +12741,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>25</v>
@@ -12203,30 +12777,56 @@
       <c r="M4" s="58" t="s">
         <v>800</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="15"/>
+      <c r="O4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="34"/>
+      <c r="M5" s="58" t="s">
+        <v>800</v>
+      </c>
+      <c r="N5" s="15" t="s">
         <v>828</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="O5" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="P5" s="15"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -12247,25 +12847,167 @@
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
     </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="mailto:santoshp@ideyalabs.com" xr:uid="{8E38F616-1BA4-4BCC-B627-DB9CF76698B0}"/>
-    <hyperlink ref="E2" r:id="rId2" display="mailto:Admin@123" xr:uid="{8765459C-FF87-43D9-9F14-0CF33CCB4D78}"/>
-    <hyperlink ref="D3" r:id="rId3" display="mailto:santoshp@ideyalabs.com" xr:uid="{D1F0AC55-866E-422A-9B3B-6A2F6F0C3CB9}"/>
-    <hyperlink ref="E3" r:id="rId4" display="mailto:Admin@123" xr:uid="{718CCB56-0571-43F4-8038-782BC675FAE3}"/>
-    <hyperlink ref="D4" r:id="rId5" display="mailto:santoshp@ideyalabs.com" xr:uid="{1556E6B5-EC05-404C-986C-4B23893AAC42}"/>
-    <hyperlink ref="E4" r:id="rId6" display="mailto:Admin@123" xr:uid="{D8B7528E-2389-4EFF-9988-878740C81CBD}"/>
+    <hyperlink ref="D3" r:id="rId1" display="mailto:santoshp@ideyalabs.com" xr:uid="{8E38F616-1BA4-4BCC-B627-DB9CF76698B0}"/>
+    <hyperlink ref="E3" r:id="rId2" display="mailto:Admin@123" xr:uid="{8765459C-FF87-43D9-9F14-0CF33CCB4D78}"/>
+    <hyperlink ref="D4" r:id="rId3" display="mailto:santoshp@ideyalabs.com" xr:uid="{D1F0AC55-866E-422A-9B3B-6A2F6F0C3CB9}"/>
+    <hyperlink ref="E4" r:id="rId4" display="mailto:Admin@123" xr:uid="{718CCB56-0571-43F4-8038-782BC675FAE3}"/>
+    <hyperlink ref="D5" r:id="rId5" display="mailto:santoshp@ideyalabs.com" xr:uid="{1556E6B5-EC05-404C-986C-4B23893AAC42}"/>
+    <hyperlink ref="E5" r:id="rId6" display="mailto:Admin@123" xr:uid="{D8B7528E-2389-4EFF-9988-878740C81CBD}"/>
+    <hyperlink ref="D2" r:id="rId7" display="mailto:santoshp@ideyalabs.com" xr:uid="{15C2FD3B-CE00-4D54-B405-C2464F6C8ED8}"/>
+    <hyperlink ref="E2" r:id="rId8" display="mailto:Admin@123" xr:uid="{AB0080EB-8230-46E9-900C-9EF418CAE849}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C2A1F7-331D-4904-8FAB-802A148F1553}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>849</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>849</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{3E132DEE-A74E-41A1-9329-92F291982AD8}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{4259E39A-C185-451B-8A14-8B051DDE43EF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D3A334-050A-4737-9B01-1B13EAAB8BDD}">
-  <dimension ref="A1:AM7"/>
+  <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AH25" sqref="AH25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12310,7 +13052,7 @@
     <col min="39" max="39" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12428,8 +13170,11 @@
       <c r="AM1" s="1" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>356</v>
       </c>
@@ -12503,7 +13248,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>375</v>
       </c>
@@ -12562,7 +13307,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>377</v>
       </c>
@@ -12600,7 +13345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>390</v>
       </c>
@@ -12653,7 +13398,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>393</v>
       </c>
@@ -12715,7 +13460,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>396</v>
       </c>
@@ -12778,6 +13523,88 @@
       </c>
       <c r="AL7" t="s">
         <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
+        <v>834</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>834</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="73" t="s">
+        <v>838</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>838</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>839</v>
       </c>
     </row>
   </sheetData>
@@ -12795,13 +13622,17 @@
     <hyperlink ref="E6" r:id="rId11" xr:uid="{8F2DF61D-1340-47C7-A580-463CCD2FE8DD}"/>
     <hyperlink ref="D7" r:id="rId12" xr:uid="{AB716087-C345-4325-BFA7-23C9C1FE83EB}"/>
     <hyperlink ref="E7" r:id="rId13" xr:uid="{E35B4D54-50AC-4384-93D1-E2D22159B4E4}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{FCE28C48-3574-4EAD-8B86-C77BC99AA3B5}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{F632E568-E786-43B2-9E7A-9480FE6C9A24}"/>
+    <hyperlink ref="D9" r:id="rId16" xr:uid="{B57504E7-818A-4A07-924F-8DF8D141D2BD}"/>
+    <hyperlink ref="E9" r:id="rId17" xr:uid="{3F883C28-0B05-420F-AF0A-71DB12880E13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F404E78-86F3-4010-B1D5-D6F63F40004D}">
   <dimension ref="A1:AH23"/>
   <sheetViews>
@@ -14565,26 +15396,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBCCE70-8886-44A0-B994-06CEF8321F97}">
-  <dimension ref="A1:AK6"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="41" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14696,13 +15528,16 @@
       <c r="AK1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>598</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>598</v>
+      <c r="AL1" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>835</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>835</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>25</v>
@@ -14728,84 +15563,43 @@
       <c r="J2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="13" t="s">
-        <v>599</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>600</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>601</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>602</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>603</v>
-      </c>
-      <c r="Q2" s="53" t="s">
-        <v>610</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>604</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>605</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>605</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>605</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="W2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>606</v>
-      </c>
-      <c r="Y2" s="15" t="s">
-        <v>607</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA2" s="27" t="s">
-        <v>608</v>
-      </c>
-      <c r="AB2" s="50" t="s">
-        <v>769</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>768</v>
-      </c>
-      <c r="AD2" s="53" t="s">
-        <v>778</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>517</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="1"/>
       <c r="AJ2" s="15"/>
-      <c r="AK2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="6" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>25</v>
@@ -14881,7 +15675,7 @@
         <v>608</v>
       </c>
       <c r="AB3" s="50" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="AC3" s="17" t="s">
         <v>768</v>
@@ -14895,28 +15689,20 @@
       <c r="AF3" s="15" t="s">
         <v>422</v>
       </c>
-      <c r="AG3" s="13" t="s">
-        <v>611</v>
-      </c>
-      <c r="AH3" s="13" t="s">
-        <v>612</v>
-      </c>
-      <c r="AI3" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="AJ3" s="15" t="s">
-        <v>613</v>
-      </c>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
       <c r="AK3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>25</v>
@@ -15022,12 +15808,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>767</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>767</v>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>614</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>25</v>
@@ -15118,10 +15904,10 @@
         <v>422</v>
       </c>
       <c r="AG5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH5" s="15" t="s">
-        <v>27</v>
+        <v>611</v>
+      </c>
+      <c r="AH5" s="13" t="s">
+        <v>612</v>
       </c>
       <c r="AI5" s="15" t="s">
         <v>430</v>
@@ -15133,41 +15919,153 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="41"/>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>767</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>767</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>600</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q6" s="53" t="s">
+        <v>610</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>604</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="W6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA6" s="27" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB6" s="50" t="s">
+        <v>770</v>
+      </c>
+      <c r="AC6" s="17" t="s">
+        <v>768</v>
+      </c>
+      <c r="AD6" s="53" t="s">
+        <v>778</v>
+      </c>
+      <c r="AE6" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="AF6" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AG6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI6" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AJ6" s="15" t="s">
+        <v>613</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1739BED2-F0C1-4EA3-8C46-0D5DA1996262}">
   <dimension ref="A1:EB2"/>
   <sheetViews>
@@ -15928,7 +16826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B5757B-1D64-4665-A795-38990E29E9FE}">
   <dimension ref="A1:R7"/>
   <sheetViews>
@@ -16306,18 +17204,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C521355-FD3D-4E65-938C-9AA1EB49CB44}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -16337,7 +17234,7 @@
     <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -16398,8 +17295,11 @@
       <c r="T1" s="1" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>418</v>
       </c>
@@ -16455,7 +17355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>459</v>
       </c>
@@ -16500,6 +17400,44 @@
       </c>
       <c r="T3" s="17" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>833</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>833</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -16508,319 +17446,9 @@
     <hyperlink ref="E2" r:id="rId2" display="mailto:Admin@123" xr:uid="{F35E9FF1-B242-4B71-A4FB-8FFB9A1948EE}"/>
     <hyperlink ref="D3" r:id="rId3" display="mailto:santoshp@ideyalabs.com" xr:uid="{189C12D3-C300-4F82-B462-B2E11831800B}"/>
     <hyperlink ref="E3" r:id="rId4" display="mailto:Admin@123" xr:uid="{861FAEC2-8A05-42B2-BC4D-CFBC5F76D40F}"/>
+    <hyperlink ref="D4" r:id="rId5" display="mailto:santoshp@ideyalabs.com" xr:uid="{7062176B-1A3A-42DE-B3D9-1071F0230B05}"/>
+    <hyperlink ref="E4" r:id="rId6" display="mailto:Admin@123" xr:uid="{78E7C5CD-7262-4BBB-BFEB-9B42504F58E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFB9E42-5696-4F0E-9E81-9692429FA356}">
-  <dimension ref="A1:AD5"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="111.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="109" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>465</v>
-      </c>
-      <c r="B2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="E2" t="s">
-        <v>491</v>
-      </c>
-      <c r="F2" t="s">
-        <v>540</v>
-      </c>
-      <c r="G2" t="s">
-        <v>541</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>542</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>474</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>475</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>488</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>487</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>498</v>
-      </c>
-      <c r="V2" s="31" t="s">
-        <v>503</v>
-      </c>
-      <c r="W2" s="57" t="s">
-        <v>803</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>801</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="AD2" s="20" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>476</v>
-      </c>
-      <c r="B3" t="s">
-        <v>477</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="E3" t="s">
-        <v>506</v>
-      </c>
-      <c r="F3" t="s">
-        <v>471</v>
-      </c>
-      <c r="G3" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>478</v>
-      </c>
-      <c r="B4" t="s">
-        <v>479</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="E4" t="s">
-        <v>484</v>
-      </c>
-      <c r="F4" t="s">
-        <v>471</v>
-      </c>
-      <c r="G4" t="s">
-        <v>472</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>490</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>474</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" t="s">
-        <v>479</v>
-      </c>
-      <c r="N4" t="s">
-        <v>482</v>
-      </c>
-      <c r="O4" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>507</v>
-      </c>
-      <c r="B5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="F5" t="s">
-        <v>471</v>
-      </c>
-      <c r="G5" t="s">
-        <v>472</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E514FC88-A5B1-4E65-87FF-7CADA1E00A73}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{3AC1157B-CBFE-4A3A-97F2-CD1BA069B9E6}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{D6C2FFC5-EEDC-4E5E-8437-BA3012C285EE}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{A4D159C9-78DA-46E9-AAA2-6DE96443BDF7}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{D01AE455-D8CC-4FA6-BD42-D57F16011A5B}"/>
-    <hyperlink ref="H2" r:id="rId6" xr:uid="{372C5DDD-5BB6-4E59-A318-BC1678609099}"/>
-    <hyperlink ref="H4" r:id="rId7" xr:uid="{FB91854F-486D-427A-88C7-1F44420EB6D5}"/>
-    <hyperlink ref="D5" r:id="rId8" xr:uid="{796B7C4B-5468-4CB8-AB33-9A2C92038486}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sanity test for Admin in qa
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-admin.xlsx
+++ b/Web/coyni/resources/testdata-admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\admin(27-12-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9558649-9895-41AA-A7B8-8A47BC4C8C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F2A007-633E-441C-918A-6C165D4FA93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coyniPortal" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3714" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="856">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2646,6 +2646,15 @@
   </si>
   <si>
     <t>VerifyBalanceReportTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify system setting </t>
+  </si>
+  <si>
+    <t>feeHeading</t>
+  </si>
+  <si>
+    <t>accountLimitHeading</t>
   </si>
 </sst>
 </file>
@@ -4666,8 +4675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB4A103-5E7C-460B-A3AA-C11BE99C8FB4}">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5447,10 +5456,10 @@
         <v>28</v>
       </c>
       <c r="X20" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y20" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -9134,10 +9143,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D290E486-9137-49B5-9733-BAB7620F9D07}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9161,10 +9170,12 @@
     <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -9225,13 +9236,22 @@
       <c r="T1" s="14" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>110</v>
+      <c r="U1" s="14" t="s">
+        <v>854</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>855</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>853</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>853</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>25</v>
@@ -9257,25 +9277,31 @@
       <c r="J2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
       <c r="T2" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>272</v>
+      </c>
+      <c r="V2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>271</v>
+        <v>109</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>271</v>
+        <v>110</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>25</v>
@@ -9301,15 +9327,11 @@
       <c r="J3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>272</v>
-      </c>
+      <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="15" t="s">
-        <v>273</v>
-      </c>
+      <c r="O3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
@@ -9318,12 +9340,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>25</v>
@@ -9349,13 +9371,15 @@
       <c r="J4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>272</v>
+      </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="15" t="s">
-        <v>275</v>
-      </c>
+      <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
+      <c r="O4" s="15" t="s">
+        <v>273</v>
+      </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
@@ -9364,12 +9388,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>25</v>
@@ -9397,10 +9421,10 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="36" t="s">
-        <v>551</v>
-      </c>
+      <c r="M5" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="N5" s="15"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
@@ -9410,12 +9434,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>25</v>
@@ -9443,10 +9467,10 @@
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="N6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="36" t="s">
+        <v>551</v>
+      </c>
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
@@ -9456,12 +9480,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>25</v>
@@ -9487,14 +9511,12 @@
       <c r="J7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="15" t="s">
-        <v>272</v>
-      </c>
+      <c r="K7" s="15"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15" t="s">
-        <v>552</v>
-      </c>
+      <c r="M7" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="N7" s="15"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
@@ -9504,12 +9526,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>543</v>
+        <v>280</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>543</v>
+        <v>276</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>25</v>
@@ -9535,33 +9557,29 @@
       <c r="J8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>272</v>
+      </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
+      <c r="N8" s="15" t="s">
+        <v>552</v>
+      </c>
       <c r="O8" s="15"/>
-      <c r="P8" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="37" t="s">
-        <v>666</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="S8" s="21" t="s">
-        <v>544</v>
-      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
       <c r="T8" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>25</v>
@@ -9598,37 +9616,89 @@
       <c r="Q9" s="37" t="s">
         <v>666</v>
       </c>
-      <c r="R9" s="21" t="s">
-        <v>546</v>
+      <c r="R9" s="15" t="s">
+        <v>463</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="T9" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
+      <c r="P10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="37" t="s">
+        <v>666</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>546</v>
+      </c>
+      <c r="S10" s="21" t="s">
+        <v>547</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10459,8 +10529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDD6E72-6031-4802-B904-6A5DCC120EE9}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10611,7 +10681,9 @@
       <c r="T2" s="59"/>
       <c r="U2" s="59"/>
       <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
+      <c r="W2" s="62" t="s">
+        <v>32</v>
+      </c>
       <c r="X2" s="61" t="s">
         <v>96</v>
       </c>
@@ -12171,7 +12243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9ECCE6-1FC9-48C7-BBB8-F3E55C223DFA}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -12582,7 +12654,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12690,7 +12762,9 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="15"/>
+      <c r="O2" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="P2" t="s">
         <v>842</v>
       </c>
@@ -15401,7 +15475,7 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AK22" sqref="AK22"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15575,7 +15649,9 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="W2" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -17208,8 +17284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C521355-FD3D-4E65-938C-9AA1EB49CB44}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17436,6 +17512,9 @@
       <c r="K4" s="15" t="s">
         <v>33</v>
       </c>
+      <c r="T4" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="U4" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Added test script for agreement TOs
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-admin.xlsx
+++ b/Web/coyni/resources/testdata-admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(02-01-2023)-Admin(2.3)encha\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB06919-9950-4ECD-BC76-28B09315E7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F837C6-DFCD-4E62-9B46-E9C277B35A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coyniPortal" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4160" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4179" uniqueCount="932">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2862,6 +2862,27 @@
   </si>
   <si>
     <t>03/02/2023</t>
+  </si>
+  <si>
+    <t>Verify  Agreements Terms of Service</t>
+  </si>
+  <si>
+    <t>Verify TOS Agreement</t>
+  </si>
+  <si>
+    <t>AgreementList</t>
+  </si>
+  <si>
+    <t>tosHeading</t>
+  </si>
+  <si>
+    <t>Id,Version,Created Date,Created By,Start Date,Effective Date,End Date,Status</t>
+  </si>
+  <si>
+    <t>coyni 2.3.pdf</t>
+  </si>
+  <si>
+    <t>Save TOS agreement</t>
   </si>
 </sst>
 </file>
@@ -9497,10 +9518,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D290E486-9137-49B5-9733-BAB7620F9D07}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Z35" sqref="Z35"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9527,9 +9548,13 @@
     <col min="20" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -9599,8 +9624,20 @@
       <c r="W1" s="14" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="14" t="s">
+        <v>927</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>852</v>
       </c>
@@ -9650,7 +9687,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>109</v>
       </c>
@@ -9694,7 +9731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>271</v>
       </c>
@@ -9742,7 +9779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>274</v>
       </c>
@@ -9788,7 +9825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>276</v>
       </c>
@@ -9834,7 +9871,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>278</v>
       </c>
@@ -9880,7 +9917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>280</v>
       </c>
@@ -9928,7 +9965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>543</v>
       </c>
@@ -9980,7 +10017,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>545</v>
       </c>
@@ -10032,17 +10069,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="s">
+        <v>925</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>926</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
@@ -10052,7 +10109,21 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
+      <c r="T11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X11" t="s">
+        <v>929</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>517</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>930</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>931</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10064,7 +10135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B863EE-0FB8-4125-A633-87E6E4517058}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
@@ -18893,7 +18964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C521355-FD3D-4E65-938C-9AA1EB49CB44}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test script for Profiles
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-admin.xlsx
+++ b/Web/coyni/resources/testdata-admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(24-03-2023)Home\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C1A41-65B1-410B-B1D5-F59AF342EF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0487379B-A645-497D-AE31-F3269FB56022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="967" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="967" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coyniPortal" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4660" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4668" uniqueCount="997">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -3077,12 +3077,15 @@
   <si>
     <t>your profile image has been successfully updated!.</t>
   </si>
+  <si>
+    <t>2341123496</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3807,11 +3810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB40DDF-741D-4E62-9E3A-43C63EE95C74}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L3" workbookViewId="0">
+    <sheetView topLeftCell="L3" workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
@@ -3837,7 +3840,7 @@
     <col min="27" max="27" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="67.5" customHeight="1">
+    <row r="2" spans="1:27" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="64.5">
+    <row r="3" spans="1:27" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -4033,7 +4036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="64.5">
+    <row r="4" spans="1:27" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -4085,7 +4088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="64.5">
+    <row r="5" spans="1:27" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="64.5">
+    <row r="6" spans="1:27" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -4167,7 +4170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>47</v>
       </c>
@@ -4224,7 +4227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>52</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>54</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>56</v>
       </c>
@@ -4395,7 +4398,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>58</v>
       </c>
@@ -4452,7 +4455,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>60</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>63</v>
       </c>
@@ -4537,7 +4540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>66</v>
       </c>
@@ -4578,7 +4581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>66</v>
       </c>
@@ -4619,7 +4622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>66</v>
       </c>
@@ -4660,7 +4663,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -4701,7 +4704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>66</v>
       </c>
@@ -4742,7 +4745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>452</v>
       </c>
@@ -4783,7 +4786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>945</v>
       </c>
@@ -4827,7 +4830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
         <v>948</v>
       </c>
@@ -4868,7 +4871,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>962</v>
       </c>
@@ -4963,7 +4966,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -4989,7 +4992,7 @@
     <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5081,7 +5084,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>462</v>
       </c>
@@ -5164,7 +5167,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>473</v>
       </c>
@@ -5187,7 +5190,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>475</v>
       </c>
@@ -5231,7 +5234,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>504</v>
       </c>
@@ -5275,7 +5278,7 @@
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
@@ -5304,7 +5307,7 @@
     <col min="27" max="27" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5387,7 +5390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>109</v>
       </c>
@@ -5433,7 +5436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="26.25">
+    <row r="3" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
@@ -5469,7 +5472,7 @@
       </c>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="26.25">
+    <row r="4" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>112</v>
       </c>
@@ -5505,7 +5508,7 @@
       </c>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="26.25">
+    <row r="5" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>112</v>
       </c>
@@ -5543,7 +5546,7 @@
       </c>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="27" thickBot="1">
+    <row r="6" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>112</v>
       </c>
@@ -5581,7 +5584,7 @@
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="27">
+    <row r="7" spans="1:27" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>123</v>
       </c>
@@ -5627,7 +5630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="82" customFormat="1">
+    <row r="8" spans="1:27" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>125</v>
       </c>
@@ -5675,7 +5678,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>125</v>
       </c>
@@ -5715,7 +5718,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
@@ -5755,7 +5758,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>125</v>
       </c>
@@ -5795,7 +5798,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>125</v>
       </c>
@@ -5835,7 +5838,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>125</v>
       </c>
@@ -5875,7 +5878,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
@@ -5915,7 +5918,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>438</v>
       </c>
@@ -5941,7 +5944,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>438</v>
       </c>
@@ -5967,7 +5970,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="16.5">
+    <row r="17" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>771</v>
       </c>
@@ -5993,7 +5996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>774</v>
       </c>
@@ -6013,7 +6016,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>782</v>
       </c>
@@ -6068,7 +6071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="73" t="s">
         <v>828</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
         <v>957</v>
       </c>
@@ -6163,7 +6166,7 @@
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -6180,7 +6183,7 @@
     <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6227,7 +6230,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
         <v>846</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>651</v>
       </c>
@@ -6306,7 +6309,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>653</v>
       </c>
@@ -6350,7 +6353,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>656</v>
       </c>
@@ -6407,7 +6410,7 @@
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" bestFit="1" customWidth="1"/>
@@ -6431,7 +6434,7 @@
     <col min="28" max="28" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6520,7 +6523,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="51.75">
+    <row r="2" spans="1:29" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>161</v>
       </c>
@@ -6585,7 +6588,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>168</v>
       </c>
@@ -6633,7 +6636,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>168</v>
       </c>
@@ -6683,7 +6686,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -6737,7 +6740,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>168</v>
       </c>
@@ -6791,7 +6794,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>168</v>
       </c>
@@ -6847,7 +6850,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>168</v>
       </c>
@@ -6905,7 +6908,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>168</v>
       </c>
@@ -6961,7 +6964,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>168</v>
       </c>
@@ -7017,7 +7020,7 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="79" t="s">
         <v>168</v>
       </c>
@@ -7075,7 +7078,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
         <v>168</v>
       </c>
@@ -7133,7 +7136,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
         <v>168</v>
       </c>
@@ -7191,7 +7194,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
         <v>168</v>
       </c>
@@ -7249,7 +7252,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="79" t="s">
         <v>168</v>
       </c>
@@ -7307,7 +7310,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>189</v>
       </c>
@@ -7353,7 +7356,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
@@ -7397,7 +7400,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>193</v>
       </c>
@@ -7443,7 +7446,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>195</v>
       </c>
@@ -7497,7 +7500,7 @@
       </c>
       <c r="AB19" s="15"/>
     </row>
-    <row r="20" spans="1:28" s="82" customFormat="1">
+    <row r="20" spans="1:28" s="82" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="79" t="s">
         <v>977</v>
       </c>
@@ -7538,7 +7541,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="79" t="s">
         <v>977</v>
       </c>
@@ -7584,7 +7587,7 @@
       <c r="Y21" s="82"/>
       <c r="Z21" s="82"/>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
         <v>977</v>
       </c>
@@ -7630,7 +7633,7 @@
       <c r="Y22" s="82"/>
       <c r="Z22" s="82"/>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
         <v>977</v>
       </c>
@@ -7676,7 +7679,7 @@
       <c r="Y23" s="82"/>
       <c r="Z23" s="82"/>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
         <v>977</v>
       </c>
@@ -7722,7 +7725,7 @@
       <c r="Y24" s="82"/>
       <c r="Z24" s="82"/>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
         <v>977</v>
       </c>
@@ -7768,7 +7771,7 @@
       <c r="Y25" s="82"/>
       <c r="Z25" s="82"/>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
         <v>977</v>
       </c>
@@ -7847,7 +7850,7 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -7868,7 +7871,7 @@
     <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -7927,7 +7930,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>508</v>
       </c>
@@ -7968,7 +7971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>510</v>
       </c>
@@ -8009,7 +8012,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>513</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>909</v>
       </c>
@@ -8093,7 +8096,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>913</v>
       </c>
@@ -8136,7 +8139,7 @@
         <v>456723</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>915</v>
       </c>
@@ -8182,7 +8185,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
         <v>958</v>
       </c>
@@ -8250,7 +8253,7 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
@@ -8272,7 +8275,7 @@
     <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8367,7 +8370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="16.5">
+    <row r="2" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>208</v>
       </c>
@@ -8440,7 +8443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="16.5">
+    <row r="3" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -8517,7 +8520,7 @@
       </c>
       <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>219</v>
       </c>
@@ -8592,7 +8595,7 @@
       </c>
       <c r="AE4" s="2"/>
     </row>
-    <row r="5" spans="1:31" ht="16.5">
+    <row r="5" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>219</v>
       </c>
@@ -8671,7 +8674,7 @@
       </c>
       <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:31" ht="39">
+    <row r="6" spans="1:31" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>219</v>
       </c>
@@ -8750,7 +8753,7 @@
       </c>
       <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:31" ht="16.5">
+    <row r="7" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>219</v>
       </c>
@@ -8827,7 +8830,7 @@
       </c>
       <c r="AE7" s="2"/>
     </row>
-    <row r="8" spans="1:31" ht="16.5">
+    <row r="8" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>219</v>
       </c>
@@ -8904,7 +8907,7 @@
       </c>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:31" ht="16.5">
+    <row r="9" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>219</v>
       </c>
@@ -8981,7 +8984,7 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
     </row>
-    <row r="10" spans="1:31" ht="16.5">
+    <row r="10" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>238</v>
       </c>
@@ -9060,7 +9063,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="16.5">
+    <row r="11" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>238</v>
       </c>
@@ -9139,7 +9142,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="16.5">
+    <row r="12" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>238</v>
       </c>
@@ -9218,7 +9221,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="16.5">
+    <row r="13" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>240</v>
       </c>
@@ -9291,7 +9294,7 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
     </row>
-    <row r="14" spans="1:31" ht="16.5">
+    <row r="14" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>240</v>
       </c>
@@ -9358,7 +9361,7 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
     </row>
-    <row r="15" spans="1:31" ht="16.5">
+    <row r="15" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>244</v>
       </c>
@@ -9429,7 +9432,7 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="79" t="s">
         <v>978</v>
       </c>
@@ -9496,7 +9499,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="16.5">
+    <row r="17" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
         <v>978</v>
       </c>
@@ -9555,7 +9558,7 @@
       <c r="AB17" s="82"/>
       <c r="AC17" s="82"/>
     </row>
-    <row r="18" spans="1:29" ht="16.5">
+    <row r="18" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="79" t="s">
         <v>978</v>
       </c>
@@ -9614,7 +9617,7 @@
       <c r="AB18" s="82"/>
       <c r="AC18" s="82"/>
     </row>
-    <row r="19" spans="1:29" ht="16.5">
+    <row r="19" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="79" t="s">
         <v>978</v>
       </c>
@@ -9673,7 +9676,7 @@
       <c r="AB19" s="82"/>
       <c r="AC19" s="82"/>
     </row>
-    <row r="20" spans="1:29" ht="16.5">
+    <row r="20" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="79" t="s">
         <v>978</v>
       </c>
@@ -9732,7 +9735,7 @@
       <c r="AB20" s="82"/>
       <c r="AC20" s="82"/>
     </row>
-    <row r="21" spans="1:29" ht="16.5">
+    <row r="21" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="79" t="s">
         <v>978</v>
       </c>
@@ -9791,7 +9794,7 @@
       <c r="AB21" s="82"/>
       <c r="AC21" s="82"/>
     </row>
-    <row r="22" spans="1:29" ht="16.5">
+    <row r="22" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="79" t="s">
         <v>978</v>
       </c>
@@ -9872,7 +9875,7 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
@@ -9902,7 +9905,7 @@
     <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -9994,7 +9997,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="47.25" customHeight="1">
+    <row r="2" spans="1:30" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>664</v>
       </c>
@@ -10075,7 +10078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>665</v>
       </c>
@@ -10122,7 +10125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>665</v>
       </c>
@@ -10167,7 +10170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="66">
+    <row r="5" spans="1:30" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>666</v>
       </c>
@@ -10227,7 +10230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="45">
+    <row r="6" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>667</v>
       </c>
@@ -10295,7 +10298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="45">
+    <row r="7" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>667</v>
       </c>
@@ -10364,7 +10367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="45">
+    <row r="8" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>667</v>
       </c>
@@ -10433,7 +10436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="45">
+    <row r="9" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>667</v>
       </c>
@@ -10502,7 +10505,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="45">
+    <row r="10" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>667</v>
       </c>
@@ -10605,7 +10608,7 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -10630,7 +10633,7 @@
     <col min="25" max="25" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -10870,7 +10873,7 @@
       </c>
       <c r="CB1" s="1"/>
     </row>
-    <row r="2" spans="1:80" ht="409.5">
+    <row r="2" spans="1:80" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>768</v>
       </c>
@@ -11114,7 +11117,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -11146,7 +11149,7 @@
     <col min="30" max="30" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -11238,7 +11241,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>849</v>
       </c>
@@ -11288,7 +11291,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>109</v>
       </c>
@@ -11332,7 +11335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>271</v>
       </c>
@@ -11380,7 +11383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>274</v>
       </c>
@@ -11426,7 +11429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>276</v>
       </c>
@@ -11487,7 +11490,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>278</v>
       </c>
@@ -11533,7 +11536,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>280</v>
       </c>
@@ -11596,7 +11599,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>540</v>
       </c>
@@ -11648,7 +11651,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>542</v>
       </c>
@@ -11700,7 +11703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="76" t="s">
         <v>922</v>
       </c>
@@ -11756,7 +11759,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="76" t="s">
         <v>929</v>
       </c>
@@ -11812,7 +11815,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
         <v>932</v>
       </c>
@@ -11882,7 +11885,7 @@
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -11912,7 +11915,7 @@
     <col min="30" max="30" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -12004,7 +12007,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>287</v>
       </c>
@@ -12066,7 +12069,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>292</v>
       </c>
@@ -12128,7 +12131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>294</v>
       </c>
@@ -12192,7 +12195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>297</v>
       </c>
@@ -12256,7 +12259,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>300</v>
       </c>
@@ -12322,7 +12325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>304</v>
       </c>
@@ -12386,7 +12389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>424</v>
       </c>
@@ -12460,7 +12463,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>449</v>
       </c>
@@ -12518,7 +12521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>454</v>
       </c>
@@ -12576,7 +12579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>533</v>
       </c>
@@ -12634,7 +12637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -12701,7 +12704,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" style="60" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" style="60" bestFit="1" customWidth="1"/>
@@ -12728,7 +12731,7 @@
     <col min="24" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -12802,7 +12805,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>839</v>
       </c>
@@ -12856,7 +12859,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="27">
+    <row r="3" spans="1:24" ht="30.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="61" t="s">
         <v>85</v>
       </c>
@@ -12927,7 +12930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
         <v>88</v>
       </c>
@@ -12998,7 +13001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
         <v>90</v>
       </c>
@@ -13069,7 +13072,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>92</v>
       </c>
@@ -13140,7 +13143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
         <v>94</v>
       </c>
@@ -13211,7 +13214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="s">
         <v>100</v>
       </c>
@@ -13282,7 +13285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
         <v>102</v>
       </c>
@@ -13375,7 +13378,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -13399,7 +13402,7 @@
     <col min="21" max="21" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -13464,7 +13467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>347</v>
       </c>
@@ -13505,7 +13508,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>348</v>
       </c>
@@ -13561,7 +13564,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>940</v>
       </c>
@@ -13617,7 +13620,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>349</v>
       </c>
@@ -13655,7 +13658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>345</v>
       </c>
@@ -13693,7 +13696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>346</v>
       </c>
@@ -13747,7 +13750,7 @@
       <selection activeCell="Z1" sqref="Z1:Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -13776,7 +13779,7 @@
     <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -13856,7 +13859,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>308</v>
       </c>
@@ -13914,7 +13917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>309</v>
       </c>
@@ -13969,7 +13972,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>310</v>
       </c>
@@ -14024,7 +14027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>311</v>
       </c>
@@ -14079,7 +14082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>312</v>
       </c>
@@ -14134,7 +14137,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>313</v>
       </c>
@@ -14197,7 +14200,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>316</v>
       </c>
@@ -14254,7 +14257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="102.75">
+    <row r="9" spans="1:26" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>318</v>
       </c>
@@ -14309,7 +14312,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="409.5">
+    <row r="10" spans="1:26" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>421</v>
       </c>
@@ -14395,7 +14398,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -14414,7 +14417,7 @@
     <col min="16" max="16" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14464,7 +14467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>943</v>
       </c>
@@ -14514,7 +14517,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>944</v>
       </c>
@@ -14577,7 +14580,7 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -14597,7 +14600,7 @@
     <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14656,7 +14659,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
         <v>848</v>
       </c>
@@ -14698,7 +14701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="74.25" customHeight="1">
+    <row r="3" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -14746,7 +14749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -14788,7 +14791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>330</v>
       </c>
@@ -14832,7 +14835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -14879,7 +14882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -14926,7 +14929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -14987,7 +14990,7 @@
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -15007,7 +15010,7 @@
     <col min="17" max="19" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15066,7 +15069,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>836</v>
       </c>
@@ -15110,7 +15113,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="114.75">
+    <row r="3" spans="1:19" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>528</v>
       </c>
@@ -15154,7 +15157,7 @@
       </c>
       <c r="P3" s="15"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>530</v>
       </c>
@@ -15198,7 +15201,7 @@
       </c>
       <c r="P4" s="15"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>531</v>
       </c>
@@ -15244,7 +15247,7 @@
       </c>
       <c r="P5" s="15"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="76" t="s">
         <v>988</v>
       </c>
@@ -15295,7 +15298,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -15335,15 +15338,16 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
@@ -15365,7 +15369,7 @@
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -15439,20 +15443,20 @@
         <v>982</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>954</v>
       </c>
       <c r="B2" t="s">
         <v>954</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F2" t="s">
@@ -15467,8 +15471,8 @@
       <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="20">
-        <v>123456</v>
+      <c r="J2" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="K2" t="s">
         <v>33</v>
@@ -15476,8 +15480,8 @@
       <c r="L2" t="s">
         <v>955</v>
       </c>
-      <c r="M2" s="20">
-        <v>123456</v>
+      <c r="M2" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="N2" t="s">
         <v>956</v>
@@ -15488,11 +15492,11 @@
       <c r="P2" t="s">
         <v>986</v>
       </c>
-      <c r="Q2" s="20">
-        <v>2341123496</v>
-      </c>
-      <c r="R2" s="20">
-        <v>123456</v>
+      <c r="Q2" s="20" t="s">
+        <v>996</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>987</v>
@@ -15517,9 +15521,11 @@
   <hyperlinks>
     <hyperlink ref="S2" r:id="rId1" xr:uid="{F0DA5371-9D9C-4786-BFFA-41A25FE93DB4}"/>
     <hyperlink ref="T2" r:id="rId2" xr:uid="{D04101F4-9BDC-472F-8E12-ED4FE53EECFE}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{DEA76D02-0FA6-4A89-AE84-2D2E6E40F8C1}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{C4D52DF3-8542-4E8A-A156-7E07A9B99B84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -15531,7 +15537,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -15548,7 +15554,7 @@
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15592,7 +15598,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>845</v>
       </c>
@@ -15649,11 +15655,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D3A334-050A-4737-9B01-1B13EAAB8BDD}">
   <dimension ref="A1:AW30"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AV10" sqref="AV10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="69" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.7109375" bestFit="1" customWidth="1"/>
@@ -15705,7 +15711,7 @@
     <col min="49" max="49" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15854,7 +15860,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>355</v>
       </c>
@@ -15927,8 +15933,11 @@
       <c r="X2" s="2" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="3" spans="1:49">
+      <c r="AA2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>374</v>
       </c>
@@ -15971,11 +15980,11 @@
       <c r="Y3" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>3</v>
+      <c r="Z3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="AB3" s="10" t="s">
         <v>50</v>
@@ -15987,7 +15996,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>376</v>
       </c>
@@ -16025,7 +16034,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -16078,7 +16087,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -16140,7 +16149,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="16.5">
+    <row r="7" spans="1:49" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>394</v>
       </c>
@@ -16205,7 +16214,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="73" t="s">
         <v>830</v>
       </c>
@@ -16246,7 +16255,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="73" t="s">
         <v>834</v>
       </c>
@@ -16287,7 +16296,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>852</v>
       </c>
@@ -16349,7 +16358,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>858</v>
       </c>
@@ -16414,7 +16423,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>858</v>
       </c>
@@ -16479,7 +16488,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>858</v>
       </c>
@@ -16544,7 +16553,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>858</v>
       </c>
@@ -16609,7 +16618,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>858</v>
       </c>
@@ -16674,7 +16683,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>858</v>
       </c>
@@ -16739,7 +16748,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="17" spans="1:49">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>858</v>
       </c>
@@ -16804,7 +16813,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="18" spans="1:49">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>858</v>
       </c>
@@ -16866,7 +16875,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>858</v>
       </c>
@@ -16928,7 +16937,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>858</v>
       </c>
@@ -16990,7 +16999,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="21" spans="1:49">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>858</v>
       </c>
@@ -17052,7 +17061,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>890</v>
       </c>
@@ -17108,7 +17117,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>899</v>
       </c>
@@ -17152,7 +17161,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>896</v>
       </c>
@@ -17196,7 +17205,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>898</v>
       </c>
@@ -17243,7 +17252,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>901</v>
       </c>
@@ -17287,7 +17296,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>904</v>
       </c>
@@ -17328,7 +17337,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>906</v>
       </c>
@@ -17384,7 +17393,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>908</v>
       </c>
@@ -17425,7 +17434,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>920</v>
       </c>
@@ -17534,11 +17543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F404E78-86F3-4010-B1D5-D6F63F40004D}">
   <dimension ref="A1:AH23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
@@ -17566,7 +17573,7 @@
     <col min="33" max="33" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75">
+    <row r="1" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -17670,7 +17677,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15.75">
+    <row r="2" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>388</v>
       </c>
@@ -17740,7 +17747,7 @@
       <c r="AG2" s="60"/>
       <c r="AH2" s="60"/>
     </row>
-    <row r="3" spans="1:34" ht="15.75">
+    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>391</v>
       </c>
@@ -17816,7 +17823,7 @@
       <c r="AG3" s="60"/>
       <c r="AH3" s="60"/>
     </row>
-    <row r="4" spans="1:34" ht="15.75">
+    <row r="4" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>391</v>
       </c>
@@ -17892,7 +17899,7 @@
       <c r="AG4" s="60"/>
       <c r="AH4" s="60"/>
     </row>
-    <row r="5" spans="1:34" ht="15.75">
+    <row r="5" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>391</v>
       </c>
@@ -17968,7 +17975,7 @@
       <c r="AG5" s="60"/>
       <c r="AH5" s="60"/>
     </row>
-    <row r="6" spans="1:34" ht="15.75">
+    <row r="6" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>391</v>
       </c>
@@ -18044,7 +18051,7 @@
       <c r="AG6" s="60"/>
       <c r="AH6" s="60"/>
     </row>
-    <row r="7" spans="1:34" ht="15.75">
+    <row r="7" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>622</v>
       </c>
@@ -18120,7 +18127,7 @@
       <c r="AG7" s="60"/>
       <c r="AH7" s="60"/>
     </row>
-    <row r="8" spans="1:34" ht="15.75">
+    <row r="8" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>394</v>
       </c>
@@ -18198,7 +18205,7 @@
       <c r="AG8" s="60"/>
       <c r="AH8" s="60"/>
     </row>
-    <row r="9" spans="1:34" ht="47.25">
+    <row r="9" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>559</v>
       </c>
@@ -18274,7 +18281,7 @@
       </c>
       <c r="AH9" s="60"/>
     </row>
-    <row r="10" spans="1:34" ht="78.75">
+    <row r="10" spans="1:34" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
         <v>564</v>
       </c>
@@ -18350,7 +18357,7 @@
       <c r="AG10" s="71"/>
       <c r="AH10" s="60"/>
     </row>
-    <row r="11" spans="1:34" ht="78.75">
+    <row r="11" spans="1:34" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
         <v>565</v>
       </c>
@@ -18426,7 +18433,7 @@
       <c r="AG11" s="71"/>
       <c r="AH11" s="60"/>
     </row>
-    <row r="12" spans="1:34" ht="78.75">
+    <row r="12" spans="1:34" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>567</v>
       </c>
@@ -18502,7 +18509,7 @@
       <c r="AG12" s="71"/>
       <c r="AH12" s="60"/>
     </row>
-    <row r="13" spans="1:34" ht="78.75">
+    <row r="13" spans="1:34" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
         <v>569</v>
       </c>
@@ -18578,7 +18585,7 @@
       <c r="AG13" s="71"/>
       <c r="AH13" s="60"/>
     </row>
-    <row r="14" spans="1:34" ht="15.75">
+    <row r="14" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
         <v>571</v>
       </c>
@@ -18644,7 +18651,7 @@
       <c r="AG14" s="71"/>
       <c r="AH14" s="60"/>
     </row>
-    <row r="15" spans="1:34" ht="15.75">
+    <row r="15" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
         <v>572</v>
       </c>
@@ -18710,7 +18717,7 @@
       <c r="AG15" s="71"/>
       <c r="AH15" s="60"/>
     </row>
-    <row r="16" spans="1:34" ht="15.75">
+    <row r="16" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
         <v>573</v>
       </c>
@@ -18776,7 +18783,7 @@
       <c r="AG16" s="71"/>
       <c r="AH16" s="60"/>
     </row>
-    <row r="17" spans="1:34" ht="15.75">
+    <row r="17" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
         <v>574</v>
       </c>
@@ -18842,7 +18849,7 @@
       <c r="AG17" s="71"/>
       <c r="AH17" s="60"/>
     </row>
-    <row r="18" spans="1:34" ht="15.75">
+    <row r="18" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
         <v>575</v>
       </c>
@@ -18908,7 +18915,7 @@
       <c r="AG18" s="71"/>
       <c r="AH18" s="60"/>
     </row>
-    <row r="19" spans="1:34" ht="15.75">
+    <row r="19" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
         <v>576</v>
       </c>
@@ -18974,7 +18981,7 @@
       <c r="AG19" s="71"/>
       <c r="AH19" s="60"/>
     </row>
-    <row r="20" spans="1:34" ht="15.75">
+    <row r="20" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>577</v>
       </c>
@@ -19040,7 +19047,7 @@
       <c r="AG20" s="71"/>
       <c r="AH20" s="60"/>
     </row>
-    <row r="21" spans="1:34" ht="15.75">
+    <row r="21" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>578</v>
       </c>
@@ -19106,7 +19113,7 @@
       <c r="AG21" s="71"/>
       <c r="AH21" s="60"/>
     </row>
-    <row r="22" spans="1:34" ht="15.75">
+    <row r="22" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
         <v>579</v>
       </c>
@@ -19174,7 +19181,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="15.75">
+    <row r="23" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
         <v>580</v>
       </c>
@@ -19302,7 +19309,7 @@
       <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
@@ -19314,7 +19321,7 @@
     <col min="38" max="38" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19430,7 +19437,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>831</v>
       </c>
@@ -19494,7 +19501,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>595</v>
       </c>
@@ -19597,7 +19604,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>606</v>
       </c>
@@ -19708,7 +19715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>611</v>
       </c>
@@ -19819,7 +19826,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>764</v>
       </c>
@@ -19930,7 +19937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
       <c r="C7" s="42"/>
@@ -19973,9 +19980,9 @@
       <selection activeCell="DS17" sqref="DS17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:132" s="22" customFormat="1">
+    <row r="1" spans="1:132" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -20373,7 +20380,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="2" spans="1:132">
+    <row r="2" spans="1:132" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>768</v>
       </c>
@@ -20734,7 +20741,7 @@
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
@@ -20755,7 +20762,7 @@
     <col min="17" max="17" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -20811,7 +20818,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="30">
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>400</v>
       </c>
@@ -20864,7 +20871,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>400</v>
       </c>
@@ -20917,7 +20924,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>405</v>
       </c>
@@ -20961,7 +20968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>405</v>
       </c>
@@ -21002,7 +21009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>405</v>
       </c>
@@ -21043,7 +21050,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>405</v>
       </c>
@@ -21112,7 +21119,7 @@
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
@@ -21134,7 +21141,7 @@
     <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -21199,7 +21206,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>416</v>
       </c>
@@ -21255,7 +21262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="45">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>457</v>
       </c>
@@ -21302,7 +21309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>829</v>
       </c>

</xml_diff>